<commit_message>
Test Case No.11 :arrow_forward: 식당 정보 확인 = :ok:  Pass
</commit_message>
<xml_diff>
--- a/Documents/Testcases.xlsx
+++ b/Documents/Testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95d95fc2871c3fdd/문서/GitHub/KNU_GLSO219001/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E53490-980E-4F33-97B2-93CEA60B5625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{56E53490-980E-4F33-97B2-93CEA60B5625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8C3EB2AC-9090-44F9-AB5D-7D1791AB989B}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{F0FBFF12-BA40-4112-8368-5FEB9255DFE4}"/>
+    <workbookView xWindow="-30" yWindow="1185" windowWidth="14400" windowHeight="8273" xr2:uid="{F0FBFF12-BA40-4112-8368-5FEB9255DFE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47578D2A-8C2A-41E1-885E-F480F1A2B15D}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -907,6 +907,9 @@
       <c r="F11" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G11" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="1">
@@ -926,6 +929,9 @@
       </c>
       <c r="F12" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="81.400000000000006" customHeight="1" x14ac:dyDescent="0.6">

</xml_diff>

<commit_message>
Test Case No.12 :arrow_forward: 즐겨찾기  = :ok:  Pass
</commit_message>
<xml_diff>
--- a/Documents/Testcases.xlsx
+++ b/Documents/Testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95d95fc2871c3fdd/문서/GitHub/KNU_GLSO219001/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{56E53490-980E-4F33-97B2-93CEA60B5625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8C3EB2AC-9090-44F9-AB5D-7D1791AB989B}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{56E53490-980E-4F33-97B2-93CEA60B5625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FAF20BE-4FC2-42C7-9C0B-A2444D67CEF9}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="1185" windowWidth="14400" windowHeight="8273" xr2:uid="{F0FBFF12-BA40-4112-8368-5FEB9255DFE4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{F0FBFF12-BA40-4112-8368-5FEB9255DFE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47578D2A-8C2A-41E1-885E-F480F1A2B15D}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -953,6 +953,9 @@
       <c r="F13" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G13" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="76.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="3">

</xml_diff>

<commit_message>
Test Case No.13 :arrow_forward: 리뷰 등록 (검증X, 리뷰 작성 평점 수정하기)
</commit_message>
<xml_diff>
--- a/Documents/Testcases.xlsx
+++ b/Documents/Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95d95fc2871c3fdd/문서/GitHub/KNU_GLSO219001/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{56E53490-980E-4F33-97B2-93CEA60B5625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FAF20BE-4FC2-42C7-9C0B-A2444D67CEF9}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{56E53490-980E-4F33-97B2-93CEA60B5625}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{061D3551-F60B-4A6A-81F8-65ECA7B11E46}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{F0FBFF12-BA40-4112-8368-5FEB9255DFE4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>No.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -649,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47578D2A-8C2A-41E1-885E-F480F1A2B15D}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -976,6 +976,9 @@
       <c r="F14" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G14" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>